<commit_message>
update on Random Forest model
</commit_message>
<xml_diff>
--- a/TiO2_sedimentation/Watertypes_data.xlsx
+++ b/TiO2_sedimentation/Watertypes_data.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vassi\Documents\GitHub\TiO2_aggregation_and_uptake\TiO2_sedimentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14C3790-3492-42E5-A748-0C3D42F22FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C480574F-EA25-4289-8E92-36D761092DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Watertypes_data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="46">
   <si>
     <t>id</t>
   </si>
@@ -155,6 +168,9 @@
   </si>
   <si>
     <t>Iso Lehmalampi</t>
+  </si>
+  <si>
+    <t>HD_diff</t>
   </si>
 </sst>
 </file>
@@ -1003,16 +1019,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1059,10 +1080,13 @@
         <v>14</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1108,11 +1132,14 @@
       <c r="O2" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="1">
+      <c r="P2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2" s="1">
         <v>0.39800000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1158,11 +1185,15 @@
       <c r="O3">
         <v>1227.25</v>
       </c>
-      <c r="P3" s="1">
+      <c r="P3">
+        <f t="shared" ref="P3:P45" si="0">O3-N3</f>
+        <v>749.74</v>
+      </c>
+      <c r="Q3" s="1">
         <v>5.96E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1208,11 +1239,15 @@
       <c r="O4">
         <v>1950.62</v>
       </c>
-      <c r="P4" s="1">
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>1041.4299999999998</v>
+      </c>
+      <c r="Q4" s="1">
         <v>0.20499999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1258,11 +1293,15 @@
       <c r="O5">
         <v>1948.86</v>
       </c>
-      <c r="P5" s="1">
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>1062.3799999999999</v>
+      </c>
+      <c r="Q5" s="1">
         <v>0.38300000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1308,11 +1347,15 @@
       <c r="O6">
         <v>1948.86</v>
       </c>
-      <c r="P6" s="1">
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>1062.3799999999999</v>
+      </c>
+      <c r="Q6" s="1">
         <v>0.66900000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1358,11 +1401,14 @@
       <c r="O7" t="s">
         <v>19</v>
       </c>
-      <c r="P7" s="1">
-        <v>6.6299999999999996E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P7" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0.39800000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1408,11 +1454,14 @@
       <c r="O8" t="s">
         <v>19</v>
       </c>
-      <c r="P8" s="1">
+      <c r="P8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q8" s="1">
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1458,11 +1507,14 @@
       <c r="O9" t="s">
         <v>19</v>
       </c>
-      <c r="P9" s="1">
+      <c r="P9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q9" s="1">
         <v>0.23100000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1508,11 +1560,14 @@
       <c r="O10" t="s">
         <v>19</v>
       </c>
-      <c r="P10" s="1">
+      <c r="P10" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10" s="1">
         <v>0.27</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1558,11 +1613,14 @@
       <c r="O11" t="s">
         <v>19</v>
       </c>
-      <c r="P11" s="1">
+      <c r="P11" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q11" s="1">
         <v>1.55E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1608,11 +1666,14 @@
       <c r="O12" t="s">
         <v>19</v>
       </c>
-      <c r="P12" s="1">
+      <c r="P12" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q12" s="1">
         <v>1.24E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1658,11 +1719,14 @@
       <c r="O13" t="s">
         <v>19</v>
       </c>
-      <c r="P13" s="1">
+      <c r="P13" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q13" s="1">
         <v>3.16E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1708,11 +1772,15 @@
       <c r="O14">
         <v>314.54000000000002</v>
       </c>
-      <c r="P14" s="1">
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>1.4800000000000182</v>
+      </c>
+      <c r="Q14" s="1">
         <v>5.7299999999999999E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1758,11 +1826,15 @@
       <c r="O15">
         <v>336.8</v>
       </c>
-      <c r="P15" s="1">
+      <c r="P15">
+        <f t="shared" si="0"/>
+        <v>5.9399999999999977</v>
+      </c>
+      <c r="Q15" s="1">
         <v>5.7299999999999999E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1808,11 +1880,15 @@
       <c r="O16">
         <v>314.54000000000002</v>
       </c>
-      <c r="P16" s="1">
+      <c r="P16">
+        <f t="shared" si="0"/>
+        <v>2.9700000000000273</v>
+      </c>
+      <c r="Q16" s="1">
         <v>5.7299999999999999E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1858,11 +1934,15 @@
       <c r="O17">
         <v>314.54000000000002</v>
       </c>
-      <c r="P17" s="1">
+      <c r="P17">
+        <f t="shared" si="0"/>
+        <v>2.9700000000000273</v>
+      </c>
+      <c r="Q17" s="1">
         <v>5.7299999999999999E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1908,11 +1988,15 @@
       <c r="O18">
         <v>251</v>
       </c>
-      <c r="P18" s="1">
+      <c r="P18">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="Q18" s="1">
         <v>1.11E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1958,11 +2042,14 @@
       <c r="O19">
         <v>228</v>
       </c>
-      <c r="P19" s="1">
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="1">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2008,11 +2095,15 @@
       <c r="O20">
         <v>548</v>
       </c>
-      <c r="P20" s="1">
+      <c r="P20">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="Q20" s="1">
         <v>1.72E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2058,11 +2149,14 @@
       <c r="O21" t="s">
         <v>19</v>
       </c>
-      <c r="P21" s="1">
+      <c r="P21" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q21" s="1">
         <v>5.7500000000000002E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2108,11 +2202,15 @@
       <c r="O22">
         <v>270</v>
       </c>
-      <c r="P22" s="1">
+      <c r="P22">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+      <c r="Q22" s="1">
         <v>1.5100000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2158,11 +2256,15 @@
       <c r="O23">
         <v>663</v>
       </c>
-      <c r="P23" s="1">
+      <c r="P23">
+        <f t="shared" si="0"/>
+        <v>469</v>
+      </c>
+      <c r="Q23" s="1">
         <v>1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2208,11 +2310,14 @@
       <c r="O24">
         <v>211</v>
       </c>
-      <c r="P24" s="1">
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="1">
         <v>2.8400000000000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2258,11 +2363,14 @@
       <c r="O25" t="s">
         <v>19</v>
       </c>
-      <c r="P25" s="1">
+      <c r="P25" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q25" s="1">
         <v>6.7900000000000002E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2308,11 +2416,15 @@
       <c r="O26">
         <v>304</v>
       </c>
-      <c r="P26" s="1">
+      <c r="P26">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="Q26" s="1">
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2358,11 +2470,15 @@
       <c r="O27">
         <v>738</v>
       </c>
-      <c r="P27" s="1">
+      <c r="P27">
+        <f t="shared" si="0"/>
+        <v>577</v>
+      </c>
+      <c r="Q27" s="1">
         <v>1.78E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2408,11 +2524,14 @@
       <c r="O28">
         <v>344</v>
       </c>
-      <c r="P28" s="1">
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="1">
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2458,11 +2577,14 @@
       <c r="O29" t="s">
         <v>19</v>
       </c>
-      <c r="P29" s="1">
+      <c r="P29" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q29" s="1">
         <v>7.5800000000000006E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2508,11 +2630,14 @@
       <c r="O30">
         <v>246</v>
       </c>
-      <c r="P30" s="1">
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="1">
         <v>1.03E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2558,11 +2683,15 @@
       <c r="O31">
         <v>514</v>
       </c>
-      <c r="P31" s="1">
+      <c r="P31">
+        <f t="shared" si="0"/>
+        <v>183</v>
+      </c>
+      <c r="Q31" s="1">
         <v>1.5699999999999999E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2608,11 +2737,14 @@
       <c r="O32">
         <v>419</v>
       </c>
-      <c r="P32" s="1">
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="1">
         <v>3.0200000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2658,11 +2790,14 @@
       <c r="O33" t="s">
         <v>19</v>
       </c>
-      <c r="P33" s="1">
+      <c r="P33" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q33" s="1">
         <v>6.4199999999999993E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2708,11 +2843,14 @@
       <c r="O34">
         <v>161</v>
       </c>
-      <c r="P34" s="1">
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="1">
         <v>1.23E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2758,11 +2896,15 @@
       <c r="O35">
         <v>514</v>
       </c>
-      <c r="P35" s="1">
+      <c r="P35">
+        <f t="shared" si="0"/>
+        <v>183</v>
+      </c>
+      <c r="Q35" s="1">
         <v>1.66E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2808,11 +2950,14 @@
       <c r="O36">
         <v>416</v>
       </c>
-      <c r="P36" s="1">
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="1">
         <v>4.0599999999999997E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2858,11 +3003,14 @@
       <c r="O37" t="s">
         <v>19</v>
       </c>
-      <c r="P37" s="1">
+      <c r="P37" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q37" s="1">
         <v>8.5900000000000004E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2908,11 +3056,15 @@
       <c r="O38">
         <v>315</v>
       </c>
-      <c r="P38" s="1">
+      <c r="P38">
+        <f t="shared" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="Q38" s="1">
         <v>1.1599999999999999E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2958,11 +3110,15 @@
       <c r="O39">
         <v>512</v>
       </c>
-      <c r="P39" s="1">
+      <c r="P39">
+        <f t="shared" si="0"/>
+        <v>137</v>
+      </c>
+      <c r="Q39" s="1">
         <v>1.43E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3008,11 +3164,14 @@
       <c r="O40">
         <v>588</v>
       </c>
-      <c r="P40" s="1">
+      <c r="P40">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="1">
         <v>2.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3058,11 +3217,14 @@
       <c r="O41" t="s">
         <v>19</v>
       </c>
-      <c r="P41" s="1">
+      <c r="P41" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q41" s="1">
         <v>8.5500000000000007E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3078,8 +3240,8 @@
       <c r="E42">
         <v>6.1</v>
       </c>
-      <c r="F42" t="s">
-        <v>19</v>
+      <c r="F42">
+        <v>292.5</v>
       </c>
       <c r="G42">
         <v>5.4</v>
@@ -3108,11 +3270,15 @@
       <c r="O42">
         <v>214.54</v>
       </c>
-      <c r="P42" s="1">
+      <c r="P42">
+        <f t="shared" si="0"/>
+        <v>4.1099999999999852</v>
+      </c>
+      <c r="Q42" s="1">
         <v>1.034243E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3128,8 +3294,8 @@
       <c r="E43">
         <v>6.1</v>
       </c>
-      <c r="F43" t="s">
-        <v>19</v>
+      <c r="F43">
+        <v>292.5</v>
       </c>
       <c r="G43">
         <v>5.4</v>
@@ -3158,11 +3324,15 @@
       <c r="O43">
         <v>1615.38</v>
       </c>
-      <c r="P43" s="1">
+      <c r="P43">
+        <f t="shared" si="0"/>
+        <v>952.15000000000009</v>
+      </c>
+      <c r="Q43" s="1">
         <v>4.3198E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3178,8 +3348,8 @@
       <c r="E44">
         <v>5</v>
       </c>
-      <c r="F44" t="s">
-        <v>19</v>
+      <c r="F44">
+        <v>292.5</v>
       </c>
       <c r="G44">
         <v>2.7</v>
@@ -3208,11 +3378,14 @@
       <c r="O44">
         <v>205.54</v>
       </c>
-      <c r="P44" s="1">
+      <c r="P44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3228,8 +3401,8 @@
       <c r="E45">
         <v>5</v>
       </c>
-      <c r="F45" t="s">
-        <v>19</v>
+      <c r="F45">
+        <v>292.5</v>
       </c>
       <c r="G45">
         <v>2.7</v>
@@ -3258,7 +3431,11 @@
       <c r="O45">
         <v>650.09</v>
       </c>
-      <c r="P45" s="1">
+      <c r="P45">
+        <f t="shared" si="0"/>
+        <v>144.46000000000004</v>
+      </c>
+      <c r="Q45" s="1">
         <v>5.2996329999999998E-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the RF model for the prediction of sedimentation rates
</commit_message>
<xml_diff>
--- a/TiO2_sedimentation/Watertypes_data.xlsx
+++ b/TiO2_sedimentation/Watertypes_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vassi\Documents\GitHub\TiO2_aggregation_and_uptake\TiO2_sedimentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C480574F-EA25-4289-8E92-36D761092DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937EAB62-3654-4756-9D98-7FDC363633F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="45">
   <si>
     <t>id</t>
   </si>
@@ -168,9 +168,6 @@
   </si>
   <si>
     <t>Iso Lehmalampi</t>
-  </si>
-  <si>
-    <t>HD_diff</t>
   </si>
 </sst>
 </file>
@@ -1019,13 +1016,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q45"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q7" sqref="Q7"/>
+      <selection pane="bottomRight" activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,7 +1030,7 @@
     <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1080,13 +1077,10 @@
         <v>14</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1132,14 +1126,11 @@
       <c r="O2" t="s">
         <v>19</v>
       </c>
-      <c r="P2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q2" s="1">
+      <c r="P2" s="1">
         <v>0.39800000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1185,15 +1176,11 @@
       <c r="O3">
         <v>1227.25</v>
       </c>
-      <c r="P3">
-        <f t="shared" ref="P3:P45" si="0">O3-N3</f>
-        <v>749.74</v>
-      </c>
-      <c r="Q3" s="1">
+      <c r="P3" s="1">
         <v>5.96E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1239,15 +1226,11 @@
       <c r="O4">
         <v>1950.62</v>
       </c>
-      <c r="P4">
-        <f t="shared" si="0"/>
-        <v>1041.4299999999998</v>
-      </c>
-      <c r="Q4" s="1">
+      <c r="P4" s="1">
         <v>0.20499999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1293,15 +1276,11 @@
       <c r="O5">
         <v>1948.86</v>
       </c>
-      <c r="P5">
-        <f t="shared" si="0"/>
-        <v>1062.3799999999999</v>
-      </c>
-      <c r="Q5" s="1">
+      <c r="P5" s="1">
         <v>0.38300000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1347,15 +1326,11 @@
       <c r="O6">
         <v>1948.86</v>
       </c>
-      <c r="P6">
-        <f t="shared" si="0"/>
-        <v>1062.3799999999999</v>
-      </c>
-      <c r="Q6" s="1">
+      <c r="P6" s="1">
         <v>0.66900000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1401,14 +1376,11 @@
       <c r="O7" t="s">
         <v>19</v>
       </c>
-      <c r="P7" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q7" s="1">
+      <c r="P7" s="1">
         <v>0.39800000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1454,14 +1426,11 @@
       <c r="O8" t="s">
         <v>19</v>
       </c>
-      <c r="P8" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q8" s="1">
+      <c r="P8" s="1">
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1507,14 +1476,11 @@
       <c r="O9" t="s">
         <v>19</v>
       </c>
-      <c r="P9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q9" s="1">
+      <c r="P9" s="1">
         <v>0.23100000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1560,14 +1526,11 @@
       <c r="O10" t="s">
         <v>19</v>
       </c>
-      <c r="P10" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q10" s="1">
+      <c r="P10" s="1">
         <v>0.27</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1613,14 +1576,11 @@
       <c r="O11" t="s">
         <v>19</v>
       </c>
-      <c r="P11" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q11" s="1">
+      <c r="P11" s="1">
         <v>1.55E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1666,14 +1626,11 @@
       <c r="O12" t="s">
         <v>19</v>
       </c>
-      <c r="P12" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q12" s="1">
+      <c r="P12" s="1">
         <v>1.24E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1719,14 +1676,11 @@
       <c r="O13" t="s">
         <v>19</v>
       </c>
-      <c r="P13" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q13" s="1">
+      <c r="P13" s="1">
         <v>3.16E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1772,15 +1726,11 @@
       <c r="O14">
         <v>314.54000000000002</v>
       </c>
-      <c r="P14">
-        <f t="shared" si="0"/>
-        <v>1.4800000000000182</v>
-      </c>
-      <c r="Q14" s="1">
+      <c r="P14" s="1">
         <v>5.7299999999999999E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1826,15 +1776,11 @@
       <c r="O15">
         <v>336.8</v>
       </c>
-      <c r="P15">
-        <f t="shared" si="0"/>
-        <v>5.9399999999999977</v>
-      </c>
-      <c r="Q15" s="1">
+      <c r="P15" s="1">
         <v>5.7299999999999999E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1880,15 +1826,11 @@
       <c r="O16">
         <v>314.54000000000002</v>
       </c>
-      <c r="P16">
-        <f t="shared" si="0"/>
-        <v>2.9700000000000273</v>
-      </c>
-      <c r="Q16" s="1">
+      <c r="P16" s="1">
         <v>5.7299999999999999E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1934,15 +1876,11 @@
       <c r="O17">
         <v>314.54000000000002</v>
       </c>
-      <c r="P17">
-        <f t="shared" si="0"/>
-        <v>2.9700000000000273</v>
-      </c>
-      <c r="Q17" s="1">
+      <c r="P17" s="1">
         <v>5.7299999999999999E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1988,15 +1926,11 @@
       <c r="O18">
         <v>251</v>
       </c>
-      <c r="P18">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="Q18" s="1">
+      <c r="P18" s="1">
         <v>1.11E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2042,14 +1976,11 @@
       <c r="O19">
         <v>228</v>
       </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="1">
+      <c r="P19" s="1">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2095,15 +2026,11 @@
       <c r="O20">
         <v>548</v>
       </c>
-      <c r="P20">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="Q20" s="1">
+      <c r="P20" s="1">
         <v>1.72E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2149,14 +2076,11 @@
       <c r="O21" t="s">
         <v>19</v>
       </c>
-      <c r="P21" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q21" s="1">
+      <c r="P21" s="1">
         <v>5.7500000000000002E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2202,15 +2126,11 @@
       <c r="O22">
         <v>270</v>
       </c>
-      <c r="P22">
-        <f t="shared" si="0"/>
-        <v>106</v>
-      </c>
-      <c r="Q22" s="1">
+      <c r="P22" s="1">
         <v>1.5100000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2256,15 +2176,11 @@
       <c r="O23">
         <v>663</v>
       </c>
-      <c r="P23">
-        <f t="shared" si="0"/>
-        <v>469</v>
-      </c>
-      <c r="Q23" s="1">
+      <c r="P23" s="1">
         <v>1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2310,14 +2226,11 @@
       <c r="O24">
         <v>211</v>
       </c>
-      <c r="P24">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="1">
+      <c r="P24" s="1">
         <v>2.8400000000000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2363,14 +2276,11 @@
       <c r="O25" t="s">
         <v>19</v>
       </c>
-      <c r="P25" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q25" s="1">
+      <c r="P25" s="1">
         <v>6.7900000000000002E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2416,15 +2326,11 @@
       <c r="O26">
         <v>304</v>
       </c>
-      <c r="P26">
-        <f t="shared" si="0"/>
-        <v>124</v>
-      </c>
-      <c r="Q26" s="1">
+      <c r="P26" s="1">
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2470,15 +2376,11 @@
       <c r="O27">
         <v>738</v>
       </c>
-      <c r="P27">
-        <f t="shared" si="0"/>
-        <v>577</v>
-      </c>
-      <c r="Q27" s="1">
+      <c r="P27" s="1">
         <v>1.78E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2524,14 +2426,11 @@
       <c r="O28">
         <v>344</v>
       </c>
-      <c r="P28">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="1">
+      <c r="P28" s="1">
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2577,14 +2476,11 @@
       <c r="O29" t="s">
         <v>19</v>
       </c>
-      <c r="P29" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q29" s="1">
+      <c r="P29" s="1">
         <v>7.5800000000000006E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2630,14 +2526,11 @@
       <c r="O30">
         <v>246</v>
       </c>
-      <c r="P30">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="1">
+      <c r="P30" s="1">
         <v>1.03E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2683,15 +2576,11 @@
       <c r="O31">
         <v>514</v>
       </c>
-      <c r="P31">
-        <f t="shared" si="0"/>
-        <v>183</v>
-      </c>
-      <c r="Q31" s="1">
+      <c r="P31" s="1">
         <v>1.5699999999999999E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2737,14 +2626,11 @@
       <c r="O32">
         <v>419</v>
       </c>
-      <c r="P32">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="1">
+      <c r="P32" s="1">
         <v>3.0200000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2790,14 +2676,11 @@
       <c r="O33" t="s">
         <v>19</v>
       </c>
-      <c r="P33" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q33" s="1">
+      <c r="P33" s="1">
         <v>6.4199999999999993E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2843,14 +2726,11 @@
       <c r="O34">
         <v>161</v>
       </c>
-      <c r="P34">
-        <v>0</v>
-      </c>
-      <c r="Q34" s="1">
+      <c r="P34" s="1">
         <v>1.23E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2896,15 +2776,11 @@
       <c r="O35">
         <v>514</v>
       </c>
-      <c r="P35">
-        <f t="shared" si="0"/>
-        <v>183</v>
-      </c>
-      <c r="Q35" s="1">
+      <c r="P35" s="1">
         <v>1.66E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2950,14 +2826,11 @@
       <c r="O36">
         <v>416</v>
       </c>
-      <c r="P36">
-        <v>0</v>
-      </c>
-      <c r="Q36" s="1">
+      <c r="P36" s="1">
         <v>4.0599999999999997E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3003,14 +2876,11 @@
       <c r="O37" t="s">
         <v>19</v>
       </c>
-      <c r="P37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q37" s="1">
+      <c r="P37" s="1">
         <v>8.5900000000000004E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3056,15 +2926,11 @@
       <c r="O38">
         <v>315</v>
       </c>
-      <c r="P38">
-        <f t="shared" si="0"/>
-        <v>86</v>
-      </c>
-      <c r="Q38" s="1">
+      <c r="P38" s="1">
         <v>1.1599999999999999E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3110,15 +2976,11 @@
       <c r="O39">
         <v>512</v>
       </c>
-      <c r="P39">
-        <f t="shared" si="0"/>
-        <v>137</v>
-      </c>
-      <c r="Q39" s="1">
+      <c r="P39" s="1">
         <v>1.43E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3164,14 +3026,11 @@
       <c r="O40">
         <v>588</v>
       </c>
-      <c r="P40">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="1">
+      <c r="P40" s="1">
         <v>2.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3217,14 +3076,11 @@
       <c r="O41" t="s">
         <v>19</v>
       </c>
-      <c r="P41" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q41" s="1">
+      <c r="P41" s="1">
         <v>8.5500000000000007E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3270,15 +3126,11 @@
       <c r="O42">
         <v>214.54</v>
       </c>
-      <c r="P42">
-        <f t="shared" si="0"/>
-        <v>4.1099999999999852</v>
-      </c>
-      <c r="Q42" s="1">
+      <c r="P42" s="1">
         <v>1.034243E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3324,15 +3176,11 @@
       <c r="O43">
         <v>1615.38</v>
       </c>
-      <c r="P43">
-        <f t="shared" si="0"/>
-        <v>952.15000000000009</v>
-      </c>
-      <c r="Q43" s="1">
+      <c r="P43" s="1">
         <v>4.3198E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3378,14 +3226,11 @@
       <c r="O44">
         <v>205.54</v>
       </c>
-      <c r="P44">
+      <c r="P44" s="1">
         <v>0</v>
       </c>
-      <c r="Q44" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3431,11 +3276,7 @@
       <c r="O45">
         <v>650.09</v>
       </c>
-      <c r="P45">
-        <f t="shared" si="0"/>
-        <v>144.46000000000004</v>
-      </c>
-      <c r="Q45" s="1">
+      <c r="P45" s="1">
         <v>5.2996329999999998E-3</v>
       </c>
     </row>

</xml_diff>